<commit_message>
updating Application Security Checklist and other Templates
</commit_message>
<xml_diff>
--- a/Templates/Application Security Checklist.xlsx
+++ b/Templates/Application Security Checklist.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://beesme-my.sharepoint.com/personal/mmahjoub_enova-me_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohit\Documents\GitProjects\Cybersecurity\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="112" documentId="13_ncr:1_{DB4D6B49-73CB-4065-B1B5-1D6F9D8A3A7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7AEAFE5-B413-47BC-AFA4-4E42D9F34985}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416"/>
   </bookViews>
   <sheets>
     <sheet name="Application Security Checklist" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Application Security Checklist'!$A$2:$E$53</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Application Security Checklist'!$A$2:$E$61</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="102">
   <si>
     <t>Input Validation</t>
   </si>
@@ -90,9 +89,6 @@
     <t>Use error handlers that do not display debugging or stack trace information</t>
   </si>
   <si>
-    <t>Implement generic error messages and use custom error pages</t>
-  </si>
-  <si>
     <t>Restrict access to logs to only authorized individuals</t>
   </si>
   <si>
@@ -151,15 +147,6 @@
   </si>
   <si>
     <t>Data at rest is encrypted</t>
-  </si>
-  <si>
-    <t>Email Use</t>
-  </si>
-  <si>
-    <t>In case of e-mail usage, the solution MUST be compliant with:
-- SPF
-- DKIM
-- DMARC</t>
   </si>
   <si>
     <t>Make sure no hardcoded credentials is in the source code</t>
@@ -236,8 +223,144 @@
     </r>
   </si>
   <si>
+    <t>Ensure logs are securely stored and monitored for suspicious activities.</t>
+  </si>
+  <si>
+    <t>Implement generic error messages and use custom error pages.
+Review error messages for leakage of sensitive information.</t>
+  </si>
+  <si>
+    <t>API Security</t>
+  </si>
+  <si>
+    <t>Ensure proper authentication and authorization on APIs.</t>
+  </si>
+  <si>
+    <t>Validate input on APIs and check for vulnerabilities such as injection.</t>
+  </si>
+  <si>
+    <t>Ensure secure communication (HTTPS) for APIs.</t>
+  </si>
+  <si>
+    <t>Automated Security Testing</t>
+  </si>
+  <si>
+    <t>Penetration Testing</t>
+  </si>
+  <si>
+    <t>Implement automated security testing tools (SCA,SAST, DAST) as part of the CI/CD pipeline.</t>
+  </si>
+  <si>
+    <t>Implement regular penetration testing for critical applications before moving to production.</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Ensure input fields do not accept null values unless explicitly allowed. Verify that inputs are properly validated on both client and server sides.</t>
+  </si>
+  <si>
+    <t>Validate and sanitize inputs to prevent special characters (e.g., &lt;, &gt;, &amp;, ', ") from being processed, which could lead to injection attacks (SQL, XSS, etc.).</t>
+  </si>
+  <si>
+    <t>Ensure inputs are restricted to a reasonable length (e.g., user name or email fields) to prevent buffer overflow and denial of service attacks.</t>
+  </si>
+  <si>
+    <t>Check that numeric inputs or date ranges are constrained to an expected range. For example, for age, ensure input values between 1 and 120.</t>
+  </si>
+  <si>
+    <t>Make sure output content is properly encoded or escaped, especially when rendering user-generated content to prevent cross-site scripting (XSS).</t>
+  </si>
+  <si>
+    <t>Ensure that inputs match the expected data type (e.g., text, number, date). Reject inputs that deviate from the expected type.</t>
+  </si>
+  <si>
+    <t>Ensure that all sensitive or private pages are protected with authentication (login) unless they are intended to be public.</t>
+  </si>
+  <si>
+    <t>Ensure password policies comply with IT security standards, requiring complexity (e.g., minimum length, use of upper/lowercase, digits, symbols) and regular password updates.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Confirm that passwords are hashed using secure algorithms (e.g., bcrypt, Argon2) before being stored. Ensure salts are used for each password.</t>
+  </si>
+  <si>
+    <t>Implement a feature that shows users their last login time and location to help them detect unauthorized access to their account.</t>
+  </si>
+  <si>
+    <t>Implement single sign-on (SSO) mechanisms using secure standards like SAML or OpenID to allow users to log in across multiple systems securely.</t>
+  </si>
+  <si>
+    <t>Ensure no passwords, API keys, or other sensitive credentials are hardcoded in the source code. Use environment variables or secure vaults.</t>
+  </si>
+  <si>
+    <t>Ensure session identifiers (tokens) are not included in URLs to avoid exposure through browser history or referrer headers.</t>
+  </si>
+  <si>
+    <t>Implement automatic session termination after a period of inactivity to prevent unauthorized access due to forgotten sessions.</t>
+  </si>
+  <si>
+    <t>Review and apply the principle of least privilege to ensure that users and systems can only access the resources they need to perform their job functions.</t>
+  </si>
+  <si>
+    <t>Ensure error messages do not reveal system information, such as server details, stack traces, or sensitive user information (user IDs, session tokens).</t>
+  </si>
+  <si>
+    <t>Replace default error messages with generic messages to avoid disclosing internal system workings.</t>
+  </si>
+  <si>
+    <t>Design custom error pages for the user and ensure error messages do not leak unnecessary details.</t>
+  </si>
+  <si>
+    <t>Ensure that access to application logs is restricted to authorized personnel only, with proper logging of any access or modifications.</t>
+  </si>
+  <si>
+    <t>Make sure that logs do not store passwords, session tokens, or any personal data unnecessarily.</t>
+  </si>
+  <si>
+    <t>Protect log files from unauthorized access and regularly monitor them for suspicious events.</t>
+  </si>
+  <si>
+    <t>Capture all successful and failed authentication attempts to detect any brute-force or unauthorized access attempts.</t>
+  </si>
+  <si>
+    <t>Review access control policies to ensure that users only have the minimal level of access needed.</t>
+  </si>
+  <si>
+    <t>Ensure proper access controls to prevent unauthorized access to server-side source code.</t>
+  </si>
+  <si>
+    <t>Ensure that sensitive information (e.g., passwords, tokens) is not transmitted via URLs in GET requests. Use POST for sensitive data.</t>
+  </si>
+  <si>
+    <t>Ensure that sensitive input fields (e.g., passwords) have auto-complete disabled to prevent sensitive data from being saved in the browser.</t>
+  </si>
+  <si>
+    <t>Ensure that any sensitive data stored on the system is encrypted using strong encryption algorithms (e.g., AES-256).</t>
+  </si>
+  <si>
+    <t>Ensure that a valid TLS certificate is installed on the server to secure communications. Self-signed certificates should be avoided.</t>
+  </si>
+  <si>
+    <t>Ensure that the application is only accessible over HTTPS and that weak encryption protocols (e.g., SSL, TLS 1.0) are disabled.</t>
+  </si>
+  <si>
+    <t>Avoid using weak or obsolete cipher suites like MD5, RC4, DES3. Only use strong encryption algorithms for data transmission.</t>
+  </si>
+  <si>
+    <t>Enable HSTS to force the browser to always connect via HTTPS, protecting against protocol downgrade attacks.</t>
+  </si>
+  <si>
+    <t>Ensure that cookies containing sensitive information are protected by the HttpOnly flag to prevent access through JavaScript.</t>
+  </si>
+  <si>
+    <t>Use the Secure flag to ensure cookies are only sent over secure HTTPS channels.</t>
+  </si>
+  <si>
+    <t>Use SameSite=strict to prevent cookies from being sent along with cross-site requests, protecting against cross-site request forgery (CSRF) attacks.</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Use the flag </t>
+      <t>Use the flag SameSite</t>
     </r>
     <r>
       <rPr>
@@ -248,7 +371,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>SameSite</t>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -258,14 +381,36 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>=strict to make sure cookie is only sent if you are currently on the site that the cookie is set for</t>
+      <t>strict policy to make sure cookie is only sent if you are currently on the site that the cookie is set for</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Ensure that the hosting provider meets security certification standards like ISO 27001 for general security or PCI DSS for payment handling applications.
+</t>
+  </si>
+  <si>
+    <t>Make Sure Security is integrated early into development cycle and on Continous basis to catch vulenarabilities early in cycle</t>
+  </si>
+  <si>
+    <t>Penetration(Automated/Manual) Should be performed before rolling out code to production to uncover any additional vulnerabilities</t>
+  </si>
+  <si>
+    <t>Ensure that all APIs enforce robust authentication mechanisms such as OAuth, JWT, or API keys to confirm the identity of the users or systems interacting with the API.</t>
+  </si>
+  <si>
+    <t>Ensure that any input received by the API, including query parameters, request bodies, and headers, is validated and sanitized</t>
+  </si>
+  <si>
+    <t>Verify that all API communication is secured using HTTPS, ensuring that data is encrypted in transit. This prevents man-in-the-middle attacks where an attacker might intercept and tamper with the data being transmitted between the client and the API server. Make sure TLS (Transport Layer Security) is implemented, and avoid outdated or insecure protocols like HTTP or SSL.</t>
+  </si>
+  <si>
+    <t>Implement generic error messages for API responses that do not expose sensitive internal details.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -475,7 +620,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -516,31 +661,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -589,6 +713,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -596,6 +729,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -699,7 +853,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp29.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -730,7 +884,31 @@
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
+<file path=xl/ctrlProps/ctrlProp36.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp37.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp38.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp39.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp40.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp41.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
@@ -761,15 +939,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>4013200</xdr:colOff>
+          <xdr:colOff>4015740</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>171450</xdr:rowOff>
+          <xdr:rowOff>175260</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
           <xdr:colOff>38100</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
+          <xdr:rowOff>15240</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -779,7 +957,7 @@
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000001040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -828,15 +1006,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>4013200</xdr:colOff>
+          <xdr:colOff>4015740</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>171450</xdr:rowOff>
+          <xdr:rowOff>175260</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
           <xdr:colOff>38100</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
+          <xdr:rowOff>15240</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -846,7 +1024,7 @@
                   <a14:compatExt spid="_x0000_s1026"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -895,15 +1073,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>4013200</xdr:colOff>
+          <xdr:colOff>4015740</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>171450</xdr:rowOff>
+          <xdr:rowOff>175260</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
           <xdr:colOff>38100</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
+          <xdr:rowOff>15240</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -913,7 +1091,7 @@
                   <a14:compatExt spid="_x0000_s1027"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -962,15 +1140,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>4013200</xdr:colOff>
+          <xdr:colOff>4015740</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>184150</xdr:rowOff>
+          <xdr:rowOff>182880</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
           <xdr:colOff>38100</xdr:colOff>
           <xdr:row>11</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:rowOff>22860</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -980,7 +1158,7 @@
                   <a14:compatExt spid="_x0000_s1028"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1029,15 +1207,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>4013200</xdr:colOff>
+          <xdr:colOff>4015740</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>171450</xdr:rowOff>
+          <xdr:rowOff>175260</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
           <xdr:colOff>38100</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
+          <xdr:rowOff>15240</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1047,7 +1225,7 @@
                   <a14:compatExt spid="_x0000_s1029"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1098,13 +1276,13 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>4000500</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>184150</xdr:rowOff>
+          <xdr:rowOff>182880</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>50800</xdr:colOff>
+          <xdr:colOff>53340</xdr:colOff>
           <xdr:row>14</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:rowOff>22860</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1114,7 +1292,7 @@
                   <a14:compatExt spid="_x0000_s1030"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1165,13 +1343,13 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>4000500</xdr:colOff>
           <xdr:row>14</xdr:row>
-          <xdr:rowOff>171450</xdr:rowOff>
+          <xdr:rowOff>175260</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>50800</xdr:colOff>
+          <xdr:colOff>53340</xdr:colOff>
           <xdr:row>16</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
+          <xdr:rowOff>15240</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1181,7 +1359,7 @@
                   <a14:compatExt spid="_x0000_s1031"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1230,15 +1408,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>4013200</xdr:colOff>
+          <xdr:colOff>4015740</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>171450</xdr:rowOff>
+          <xdr:rowOff>175260</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
           <xdr:colOff>38100</xdr:colOff>
           <xdr:row>17</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
+          <xdr:rowOff>15240</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1248,7 +1426,7 @@
                   <a14:compatExt spid="_x0000_s1032"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1299,13 +1477,13 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>4000500</xdr:colOff>
           <xdr:row>16</xdr:row>
-          <xdr:rowOff>184150</xdr:rowOff>
+          <xdr:rowOff>182880</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>50800</xdr:colOff>
+          <xdr:colOff>53340</xdr:colOff>
           <xdr:row>18</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:rowOff>22860</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1315,7 +1493,7 @@
                   <a14:compatExt spid="_x0000_s1034"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1366,13 +1544,13 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>4000500</xdr:colOff>
           <xdr:row>17</xdr:row>
-          <xdr:rowOff>184150</xdr:rowOff>
+          <xdr:rowOff>182880</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>50800</xdr:colOff>
+          <xdr:colOff>53340</xdr:colOff>
           <xdr:row>19</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:rowOff>22860</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1382,7 +1560,7 @@
                   <a14:compatExt spid="_x0000_s1035"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1433,13 +1611,13 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>4000500</xdr:colOff>
           <xdr:row>21</xdr:row>
-          <xdr:rowOff>171450</xdr:rowOff>
+          <xdr:rowOff>175260</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>50800</xdr:colOff>
+          <xdr:colOff>53340</xdr:colOff>
           <xdr:row>23</xdr:row>
-          <xdr:rowOff>12700</xdr:rowOff>
+          <xdr:rowOff>15240</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1449,7 +1627,7 @@
                   <a14:compatExt spid="_x0000_s1036"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1500,13 +1678,13 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>4000500</xdr:colOff>
           <xdr:row>22</xdr:row>
-          <xdr:rowOff>165100</xdr:rowOff>
+          <xdr:rowOff>167640</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>50800</xdr:colOff>
+          <xdr:colOff>53340</xdr:colOff>
           <xdr:row>23</xdr:row>
-          <xdr:rowOff>184150</xdr:rowOff>
+          <xdr:rowOff>182880</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1516,7 +1694,7 @@
                   <a14:compatExt spid="_x0000_s1037"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1565,15 +1743,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>4013200</xdr:colOff>
+          <xdr:colOff>4015740</xdr:colOff>
           <xdr:row>25</xdr:row>
-          <xdr:rowOff>69850</xdr:rowOff>
+          <xdr:rowOff>68580</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
           <xdr:colOff>38100</xdr:colOff>
           <xdr:row>25</xdr:row>
-          <xdr:rowOff>285750</xdr:rowOff>
+          <xdr:rowOff>289560</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1583,7 +1761,7 @@
                   <a14:compatExt spid="_x0000_s1038"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1634,13 +1812,13 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>27</xdr:row>
-          <xdr:rowOff>222250</xdr:rowOff>
+          <xdr:rowOff>220980</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>50800</xdr:colOff>
+          <xdr:colOff>53340</xdr:colOff>
           <xdr:row>27</xdr:row>
-          <xdr:rowOff>368300</xdr:rowOff>
+          <xdr:rowOff>365760</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1650,7 +1828,7 @@
                   <a14:compatExt spid="_x0000_s1039"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1701,13 +1879,13 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>4000500</xdr:colOff>
           <xdr:row>28</xdr:row>
-          <xdr:rowOff>107950</xdr:rowOff>
+          <xdr:rowOff>106680</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>50800</xdr:colOff>
+          <xdr:colOff>53340</xdr:colOff>
           <xdr:row>28</xdr:row>
-          <xdr:rowOff>323850</xdr:rowOff>
+          <xdr:rowOff>327660</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1717,7 +1895,7 @@
                   <a14:compatExt spid="_x0000_s1040"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000010040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1766,15 +1944,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>4013200</xdr:colOff>
+          <xdr:colOff>4015740</xdr:colOff>
           <xdr:row>29</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>50800</xdr:colOff>
-          <xdr:row>30</xdr:row>
-          <xdr:rowOff>31750</xdr:rowOff>
+          <xdr:colOff>53340</xdr:colOff>
+          <xdr:row>29</xdr:row>
+          <xdr:rowOff>214630</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1784,7 +1962,7 @@
                   <a14:compatExt spid="_x0000_s1041"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000011040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1833,15 +2011,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>4013200</xdr:colOff>
+          <xdr:colOff>4015740</xdr:colOff>
           <xdr:row>29</xdr:row>
           <xdr:rowOff>190500</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
           <xdr:colOff>38100</xdr:colOff>
-          <xdr:row>31</xdr:row>
-          <xdr:rowOff>31750</xdr:rowOff>
+          <xdr:row>30</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1851,7 +2029,7 @@
                   <a14:compatExt spid="_x0000_s1042"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000012040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1900,15 +2078,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>4013200</xdr:colOff>
-          <xdr:row>31</xdr:row>
+          <xdr:colOff>4015740</xdr:colOff>
+          <xdr:row>32</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>50800</xdr:colOff>
-          <xdr:row>31</xdr:row>
-          <xdr:rowOff>336550</xdr:rowOff>
+          <xdr:colOff>53340</xdr:colOff>
+          <xdr:row>32</xdr:row>
+          <xdr:rowOff>335280</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1918,7 +2096,7 @@
                   <a14:compatExt spid="_x0000_s1043"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000013040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1967,15 +2145,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>4013200</xdr:colOff>
-          <xdr:row>31</xdr:row>
+          <xdr:colOff>4015740</xdr:colOff>
+          <xdr:row>32</xdr:row>
           <xdr:rowOff>381000</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
           <xdr:colOff>38100</xdr:colOff>
-          <xdr:row>33</xdr:row>
-          <xdr:rowOff>31750</xdr:rowOff>
+          <xdr:row>34</xdr:row>
+          <xdr:rowOff>30480</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1985,7 +2163,7 @@
                   <a14:compatExt spid="_x0000_s1044"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000014040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2034,15 +2212,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>4013200</xdr:colOff>
-          <xdr:row>34</xdr:row>
-          <xdr:rowOff>209550</xdr:rowOff>
+          <xdr:colOff>4015740</xdr:colOff>
+          <xdr:row>35</xdr:row>
+          <xdr:rowOff>213360</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>50800</xdr:colOff>
-          <xdr:row>34</xdr:row>
-          <xdr:rowOff>368300</xdr:rowOff>
+          <xdr:colOff>53340</xdr:colOff>
+          <xdr:row>36</xdr:row>
+          <xdr:rowOff>2345</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2052,7 +2230,7 @@
                   <a14:compatExt spid="_x0000_s1045"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000015040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2101,15 +2279,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>4019550</xdr:colOff>
-          <xdr:row>35</xdr:row>
-          <xdr:rowOff>69850</xdr:rowOff>
+          <xdr:colOff>4023360</xdr:colOff>
+          <xdr:row>36</xdr:row>
+          <xdr:rowOff>68580</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>44450</xdr:colOff>
-          <xdr:row>35</xdr:row>
-          <xdr:rowOff>184150</xdr:rowOff>
+          <xdr:colOff>45720</xdr:colOff>
+          <xdr:row>36</xdr:row>
+          <xdr:rowOff>182880</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2119,7 +2297,7 @@
                   <a14:compatExt spid="_x0000_s1046"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000016040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2169,14 +2347,14 @@
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>36</xdr:row>
-          <xdr:rowOff>95250</xdr:rowOff>
+          <xdr:row>37</xdr:row>
+          <xdr:rowOff>99060</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
           <xdr:colOff>38100</xdr:colOff>
-          <xdr:row>36</xdr:row>
-          <xdr:rowOff>292100</xdr:rowOff>
+          <xdr:row>37</xdr:row>
+          <xdr:rowOff>289560</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2186,7 +2364,7 @@
                   <a14:compatExt spid="_x0000_s1047"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000017040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2235,15 +2413,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>4013200</xdr:colOff>
-          <xdr:row>37</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
+          <xdr:colOff>4015740</xdr:colOff>
+          <xdr:row>38</xdr:row>
+          <xdr:rowOff>60960</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
           <xdr:colOff>38100</xdr:colOff>
-          <xdr:row>37</xdr:row>
-          <xdr:rowOff>279400</xdr:rowOff>
+          <xdr:row>38</xdr:row>
+          <xdr:rowOff>281940</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2253,7 +2431,7 @@
                   <a14:compatExt spid="_x0000_s1048"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000018040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2308,9 +2486,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>50800</xdr:colOff>
+          <xdr:colOff>53340</xdr:colOff>
           <xdr:row>20</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:rowOff>22860</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2320,7 +2498,7 @@
                   <a14:compatExt spid="_x0000_s1050"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2370,14 +2548,14 @@
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>38</xdr:row>
+          <xdr:row>39</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>50800</xdr:colOff>
-          <xdr:row>39</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:colOff>53340</xdr:colOff>
+          <xdr:row>40</xdr:row>
+          <xdr:rowOff>22860</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2387,7 +2565,7 @@
                   <a14:compatExt spid="_x0000_s1051"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001B040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2437,14 +2615,14 @@
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>39</xdr:row>
-          <xdr:rowOff>165100</xdr:rowOff>
+          <xdr:row>40</xdr:row>
+          <xdr:rowOff>167640</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
           <xdr:colOff>38100</xdr:colOff>
-          <xdr:row>41</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:row>42</xdr:row>
+          <xdr:rowOff>22860</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2454,7 +2632,7 @@
                   <a14:compatExt spid="_x0000_s1054"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2504,14 +2682,14 @@
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>46</xdr:row>
-          <xdr:rowOff>165100</xdr:rowOff>
+          <xdr:row>47</xdr:row>
+          <xdr:rowOff>167640</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
           <xdr:colOff>38100</xdr:colOff>
-          <xdr:row>47</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:row>48</xdr:row>
+          <xdr:rowOff>22860</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2521,7 +2699,7 @@
                   <a14:compatExt spid="_x0000_s1055"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001F040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2571,14 +2749,14 @@
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>47</xdr:row>
-          <xdr:rowOff>165100</xdr:rowOff>
+          <xdr:row>48</xdr:row>
+          <xdr:rowOff>167640</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
           <xdr:colOff>38100</xdr:colOff>
-          <xdr:row>48</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:row>49</xdr:row>
+          <xdr:rowOff>22860</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2588,7 +2766,7 @@
                   <a14:compatExt spid="_x0000_s1056"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000020040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2645,7 +2823,7 @@
           <xdr:col>3</xdr:col>
           <xdr:colOff>38100</xdr:colOff>
           <xdr:row>21</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:rowOff>22860</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2655,7 +2833,7 @@
                   <a14:compatExt spid="_x0000_s1060"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000024040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000024040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2705,14 +2883,14 @@
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>41</xdr:row>
-          <xdr:rowOff>139700</xdr:rowOff>
+          <xdr:row>42</xdr:row>
+          <xdr:rowOff>137160</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
           <xdr:colOff>38100</xdr:colOff>
-          <xdr:row>41</xdr:row>
-          <xdr:rowOff>336550</xdr:rowOff>
+          <xdr:row>42</xdr:row>
+          <xdr:rowOff>335280</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2722,7 +2900,7 @@
                   <a14:compatExt spid="_x0000_s1061"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000025040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000025040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2772,14 +2950,14 @@
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>42</xdr:row>
-          <xdr:rowOff>165100</xdr:rowOff>
+          <xdr:row>43</xdr:row>
+          <xdr:rowOff>167640</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
           <xdr:colOff>38100</xdr:colOff>
-          <xdr:row>42</xdr:row>
-          <xdr:rowOff>387350</xdr:rowOff>
+          <xdr:row>43</xdr:row>
+          <xdr:rowOff>388620</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2789,7 +2967,7 @@
                   <a14:compatExt spid="_x0000_s1062"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000026040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000026040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2839,14 +3017,14 @@
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>45</xdr:row>
-          <xdr:rowOff>165100</xdr:rowOff>
+          <xdr:row>46</xdr:row>
+          <xdr:rowOff>167640</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
           <xdr:colOff>38100</xdr:colOff>
-          <xdr:row>46</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:row>47</xdr:row>
+          <xdr:rowOff>22860</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2856,7 +3034,7 @@
                   <a14:compatExt spid="_x0000_s1063"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000027040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000027040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2906,14 +3084,14 @@
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>43</xdr:row>
-          <xdr:rowOff>165100</xdr:rowOff>
+          <xdr:row>44</xdr:row>
+          <xdr:rowOff>167640</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
           <xdr:colOff>38100</xdr:colOff>
-          <xdr:row>44</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:row>45</xdr:row>
+          <xdr:rowOff>22860</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2923,7 +3101,7 @@
                   <a14:compatExt spid="_x0000_s1064"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000028040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000028040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2969,28 +3147,23 @@
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
+      <xdr:oneCellAnchor>
         <xdr:from>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
-          <xdr:row>49</xdr:row>
-          <xdr:rowOff>165100</xdr:rowOff>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>4015740</xdr:colOff>
+          <xdr:row>31</xdr:row>
+          <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
-        <xdr:to>
-          <xdr:col>3</xdr:col>
-          <xdr:colOff>38100</xdr:colOff>
-          <xdr:row>49</xdr:row>
-          <xdr:rowOff>393700</xdr:rowOff>
-        </xdr:to>
+        <xdr:ext cx="513080" cy="220980"/>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1065" name="Check Box 41" descr="&#10;" hidden="1">
+            <xdr:cNvPr id="1072" name="Check Box 48" descr="&#10;" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1065"/>
+                  <a14:compatExt spid="_x0000_s1072"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000029040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000013040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3030,6 +3203,70 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>6350</xdr:colOff>
+          <xdr:row>49</xdr:row>
+          <xdr:rowOff>148590</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>44450</xdr:colOff>
+          <xdr:row>51</xdr:row>
+          <xdr:rowOff>3810</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1073" name="Check Box 49" descr="&#10;" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1073"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
       </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
@@ -3039,25 +3276,338 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:colOff>13970</xdr:colOff>
+          <xdr:row>50</xdr:row>
+          <xdr:rowOff>171450</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>52070</xdr:colOff>
+          <xdr:row>52</xdr:row>
+          <xdr:rowOff>26670</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1074" name="Check Box 50" descr="&#10;" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1074"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>20320</xdr:colOff>
           <xdr:row>51</xdr:row>
           <xdr:rowOff>165100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>38100</xdr:colOff>
-          <xdr:row>51</xdr:row>
-          <xdr:rowOff>387350</xdr:rowOff>
+          <xdr:colOff>58420</xdr:colOff>
+          <xdr:row>53</xdr:row>
+          <xdr:rowOff>20320</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1066" name="Check Box 42" descr="&#10;" hidden="1">
+            <xdr:cNvPr id="1075" name="Check Box 51" descr="&#10;" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1066"/>
+                  <a14:compatExt spid="_x0000_s1075"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>45720</xdr:colOff>
+          <xdr:row>52</xdr:row>
+          <xdr:rowOff>177800</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>83820</xdr:colOff>
+          <xdr:row>53</xdr:row>
+          <xdr:rowOff>217170</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1076" name="Check Box 52" descr="&#10;" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1076"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>11724</xdr:colOff>
+          <xdr:row>59</xdr:row>
+          <xdr:rowOff>67994</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="495300" cy="220980"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1078" name="Check Box 54" descr="&#10;" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1078"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002A040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002A040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>57</xdr:row>
+          <xdr:rowOff>167640</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="495300" cy="220980"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1079" name="Check Box 55" descr="&#10;" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1079"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002A040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>55</xdr:row>
+          <xdr:rowOff>167640</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>38100</xdr:colOff>
+          <xdr:row>55</xdr:row>
+          <xdr:rowOff>388620</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1080" name="Check Box 56" descr="&#10;" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1080"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3366,71 +3916,76 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:D52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A2:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A50" zoomScale="120" zoomScaleNormal="130" zoomScaleSheetLayoutView="120" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="120" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.453125" customWidth="1"/>
-    <col min="3" max="3" width="6.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.54296875" customWidth="1"/>
+    <col min="1" max="1" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.44140625" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" customWidth="1"/>
+    <col min="5" max="5" width="46.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-    </row>
-    <row r="3" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="30"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-    </row>
-    <row r="4" spans="1:4" ht="4.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="32"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="35"/>
-    </row>
-    <row r="5" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+    </row>
+    <row r="3" spans="1:5" ht="18.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+    </row>
+    <row r="4" spans="1:5" ht="4.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="25"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="28"/>
+    </row>
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="1:5" ht="5.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="29"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="32"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
         <v>34</v>
-      </c>
-      <c r="D5" s="6"/>
-    </row>
-    <row r="6" spans="1:4" ht="5.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="36"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="39"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="9" t="s">
-        <v>35</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="25" t="s">
+      <c r="E7" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -3438,46 +3993,61 @@
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="25"/>
+      <c r="E8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="18"/>
       <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="25"/>
+      <c r="E9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="18"/>
       <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="25"/>
+      <c r="E10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="18"/>
       <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="25"/>
+      <c r="E11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="18"/>
       <c r="B12" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="16"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="18"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="33"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="35"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>1</v>
       </c>
@@ -3486,15 +4056,18 @@
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="16"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="18"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="25" t="s">
+      <c r="E14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="33"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="35"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="18" t="s">
         <v>2</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -3502,55 +4075,73 @@
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="25"/>
+      <c r="E16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="18"/>
       <c r="B17" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="25"/>
+      <c r="E17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="18"/>
       <c r="B18" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="25"/>
+      <c r="E18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="18"/>
       <c r="B19" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="25"/>
+      <c r="E19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="18"/>
       <c r="B20" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="25"/>
+      <c r="E20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="18"/>
       <c r="B21" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="16"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="18"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="25" t="s">
+      <c r="E21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="33"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="35"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="18" t="s">
         <v>3</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -3558,24 +4149,30 @@
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="25"/>
+      <c r="E23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="18"/>
       <c r="B24" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="4"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" s="40" t="s">
+      <c r="E24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="41"/>
-      <c r="C25" s="41"/>
-      <c r="D25" s="42"/>
-    </row>
-    <row r="26" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="B25" s="37"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="38"/>
+    </row>
+    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>4</v>
       </c>
@@ -3584,224 +4181,377 @@
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="4"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="16"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="18"/>
-    </row>
-    <row r="28" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="25" t="s">
-        <v>24</v>
+      <c r="E26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="33"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="35"/>
+    </row>
+    <row r="28" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="18" t="s">
+        <v>23</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A29" s="25"/>
+      <c r="E28" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="18"/>
       <c r="B29" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="25"/>
+      <c r="E29" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="18"/>
       <c r="B30" s="2" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="4"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" s="25"/>
+      <c r="E30" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="18"/>
       <c r="B31" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="4"/>
-    </row>
-    <row r="32" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="25"/>
+      <c r="E31" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="18"/>
       <c r="B32" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="4"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" s="25"/>
+      <c r="E32" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="18"/>
       <c r="B33" s="2" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="4"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" s="16"/>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="18"/>
-    </row>
-    <row r="35" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C35" s="3"/>
-      <c r="D35" s="4"/>
-    </row>
-    <row r="36" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="20"/>
+      <c r="E33" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="18"/>
+      <c r="B34" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="4"/>
+      <c r="E34" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="33"/>
+      <c r="B35" s="34"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="35"/>
+    </row>
+    <row r="36" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="39" t="s">
+        <v>29</v>
+      </c>
       <c r="B36" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="4"/>
-    </row>
-    <row r="37" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A37" s="20"/>
+      <c r="E36" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="40"/>
       <c r="B37" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="4"/>
-    </row>
-    <row r="38" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="20"/>
+      <c r="E37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="40"/>
       <c r="B38" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="4"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" s="21"/>
-      <c r="B39" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C39" s="14"/>
-      <c r="D39" s="15"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" s="31"/>
-      <c r="B40" s="31"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C41" s="3"/>
-      <c r="D41" s="4"/>
-    </row>
-    <row r="42" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="27"/>
+      <c r="E38" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="40"/>
+      <c r="B39" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C39" s="3"/>
+      <c r="D39" s="4"/>
+      <c r="E39" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="41"/>
+      <c r="B40" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C40" s="14"/>
+      <c r="D40" s="15"/>
+      <c r="E40" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="24"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="24"/>
+      <c r="D41" s="24"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="19" t="s">
+        <v>36</v>
+      </c>
       <c r="B42" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="4"/>
-    </row>
-    <row r="43" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A43" s="27"/>
+      <c r="E42" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A43" s="20"/>
       <c r="B43" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="4"/>
-    </row>
-    <row r="44" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="28"/>
+      <c r="E43" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A44" s="20"/>
       <c r="B44" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="4"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A45" s="16"/>
-      <c r="B45" s="17"/>
-      <c r="C45" s="17"/>
-      <c r="D45" s="18"/>
-    </row>
-    <row r="46" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A46" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C46" s="3"/>
-      <c r="D46" s="4"/>
-    </row>
-    <row r="47" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A47" s="23"/>
+      <c r="E44" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="21"/>
+      <c r="B45" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C45" s="3"/>
+      <c r="D45" s="4"/>
+      <c r="E45" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="33"/>
+      <c r="B46" s="34"/>
+      <c r="C46" s="34"/>
+      <c r="D46" s="35"/>
+    </row>
+    <row r="47" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A47" s="42" t="s">
+        <v>38</v>
+      </c>
       <c r="B47" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="4"/>
-    </row>
-    <row r="48" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A48" s="24"/>
+      <c r="E47" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A48" s="43"/>
       <c r="B48" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="4"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A49" s="16"/>
-      <c r="B49" s="17"/>
-      <c r="C49" s="17"/>
-      <c r="D49" s="18"/>
-    </row>
-    <row r="50" spans="1:4" ht="58" x14ac:dyDescent="0.35">
-      <c r="A50" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C50" s="3"/>
-      <c r="D50" s="4"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A51" s="16"/>
-      <c r="B51" s="17"/>
-      <c r="C51" s="17"/>
-      <c r="D51" s="18"/>
-    </row>
-    <row r="52" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A52" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>48</v>
+      <c r="E48" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A49" s="44"/>
+      <c r="B49" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C49" s="3"/>
+      <c r="D49" s="4"/>
+      <c r="E49" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="33"/>
+      <c r="B50" s="34"/>
+      <c r="C50" s="34"/>
+      <c r="D50" s="35"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C51" s="3"/>
+      <c r="D51" s="4"/>
+      <c r="E51" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="20"/>
+      <c r="B52" t="s">
+        <v>53</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="4"/>
+      <c r="E52" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="20"/>
+      <c r="B53" t="s">
+        <v>54</v>
+      </c>
+      <c r="C53" s="3"/>
+      <c r="D53" s="4"/>
+      <c r="E53" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A54" s="21"/>
+      <c r="B54" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C54" s="3"/>
+      <c r="D54" s="4"/>
+      <c r="E54" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" s="33"/>
+      <c r="B55" s="34"/>
+      <c r="C55" s="34"/>
+      <c r="D55" s="35"/>
+    </row>
+    <row r="56" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A56" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C56" s="3"/>
+      <c r="D56" s="4"/>
+      <c r="E56" s="45" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" s="33"/>
+      <c r="B57" s="34"/>
+      <c r="C57" s="34"/>
+      <c r="D57" s="35"/>
+    </row>
+    <row r="58" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A58" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C58" s="3"/>
+      <c r="D58" s="4"/>
+      <c r="E58" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" s="33"/>
+      <c r="B59" s="34"/>
+      <c r="C59" s="34"/>
+      <c r="D59" s="35"/>
+    </row>
+    <row r="60" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A60" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C60" s="3"/>
+      <c r="D60" s="4"/>
+      <c r="E60" t="s">
+        <v>97</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="23">
+    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A50:D50"/>
+    <mergeCell ref="A36:A40"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A51:A54"/>
     <mergeCell ref="A16:A21"/>
-    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A42:A45"/>
     <mergeCell ref="A2:D3"/>
-    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A41:D41"/>
     <mergeCell ref="A8:A12"/>
     <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A28:A33"/>
+    <mergeCell ref="A28:A34"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="A6:D6"/>
     <mergeCell ref="A13:D13"/>
@@ -3809,15 +4559,10 @@
     <mergeCell ref="A22:D22"/>
     <mergeCell ref="A25:D25"/>
     <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="A51:D51"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="A49:D49"/>
-    <mergeCell ref="A35:A39"/>
-    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="A35:D35"/>
   </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="D5" xr:uid="{AF59408E-E4CA-4DC4-9D59-F5289A7A39C0}">
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="date" operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="D5">
       <formula1>43831</formula1>
     </dataValidation>
   </dataValidations>
@@ -3835,15 +4580,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>4013200</xdr:colOff>
+                    <xdr:colOff>4015740</xdr:colOff>
                     <xdr:row>6</xdr:row>
-                    <xdr:rowOff>171450</xdr:rowOff>
+                    <xdr:rowOff>175260</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>38100</xdr:colOff>
                     <xdr:row>8</xdr:row>
-                    <xdr:rowOff>12700</xdr:rowOff>
+                    <xdr:rowOff>15240</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3857,15 +4602,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>4013200</xdr:colOff>
+                    <xdr:colOff>4015740</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>171450</xdr:rowOff>
+                    <xdr:rowOff>175260</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>38100</xdr:colOff>
                     <xdr:row>9</xdr:row>
-                    <xdr:rowOff>12700</xdr:rowOff>
+                    <xdr:rowOff>15240</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3879,15 +4624,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>4013200</xdr:colOff>
+                    <xdr:colOff>4015740</xdr:colOff>
                     <xdr:row>8</xdr:row>
-                    <xdr:rowOff>171450</xdr:rowOff>
+                    <xdr:rowOff>175260</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>38100</xdr:colOff>
                     <xdr:row>10</xdr:row>
-                    <xdr:rowOff>12700</xdr:rowOff>
+                    <xdr:rowOff>15240</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3901,15 +4646,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>4013200</xdr:colOff>
+                    <xdr:colOff>4015740</xdr:colOff>
                     <xdr:row>9</xdr:row>
-                    <xdr:rowOff>184150</xdr:rowOff>
+                    <xdr:rowOff>182880</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>38100</xdr:colOff>
                     <xdr:row>11</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:rowOff>22860</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3923,15 +4668,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>4013200</xdr:colOff>
+                    <xdr:colOff>4015740</xdr:colOff>
                     <xdr:row>10</xdr:row>
-                    <xdr:rowOff>171450</xdr:rowOff>
+                    <xdr:rowOff>175260</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>38100</xdr:colOff>
                     <xdr:row>12</xdr:row>
-                    <xdr:rowOff>12700</xdr:rowOff>
+                    <xdr:rowOff>15240</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3947,13 +4692,13 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>4000500</xdr:colOff>
                     <xdr:row>12</xdr:row>
-                    <xdr:rowOff>184150</xdr:rowOff>
+                    <xdr:rowOff>182880</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>50800</xdr:colOff>
+                    <xdr:colOff>53340</xdr:colOff>
                     <xdr:row>14</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:rowOff>22860</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3969,13 +4714,13 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>4000500</xdr:colOff>
                     <xdr:row>14</xdr:row>
-                    <xdr:rowOff>171450</xdr:rowOff>
+                    <xdr:rowOff>175260</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>50800</xdr:colOff>
+                    <xdr:colOff>53340</xdr:colOff>
                     <xdr:row>16</xdr:row>
-                    <xdr:rowOff>12700</xdr:rowOff>
+                    <xdr:rowOff>15240</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3989,15 +4734,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>4013200</xdr:colOff>
+                    <xdr:colOff>4015740</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>171450</xdr:rowOff>
+                    <xdr:rowOff>175260</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>38100</xdr:colOff>
                     <xdr:row>17</xdr:row>
-                    <xdr:rowOff>12700</xdr:rowOff>
+                    <xdr:rowOff>15240</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4013,13 +4758,13 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>4000500</xdr:colOff>
                     <xdr:row>16</xdr:row>
-                    <xdr:rowOff>184150</xdr:rowOff>
+                    <xdr:rowOff>182880</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>50800</xdr:colOff>
+                    <xdr:colOff>53340</xdr:colOff>
                     <xdr:row>18</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:rowOff>22860</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4035,13 +4780,13 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>4000500</xdr:colOff>
                     <xdr:row>17</xdr:row>
-                    <xdr:rowOff>184150</xdr:rowOff>
+                    <xdr:rowOff>182880</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>50800</xdr:colOff>
+                    <xdr:colOff>53340</xdr:colOff>
                     <xdr:row>19</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:rowOff>22860</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4057,13 +4802,13 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>4000500</xdr:colOff>
                     <xdr:row>21</xdr:row>
-                    <xdr:rowOff>171450</xdr:rowOff>
+                    <xdr:rowOff>175260</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>50800</xdr:colOff>
+                    <xdr:colOff>53340</xdr:colOff>
                     <xdr:row>23</xdr:row>
-                    <xdr:rowOff>12700</xdr:rowOff>
+                    <xdr:rowOff>15240</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4079,13 +4824,13 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>4000500</xdr:colOff>
                     <xdr:row>22</xdr:row>
-                    <xdr:rowOff>165100</xdr:rowOff>
+                    <xdr:rowOff>167640</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>50800</xdr:colOff>
+                    <xdr:colOff>53340</xdr:colOff>
                     <xdr:row>23</xdr:row>
-                    <xdr:rowOff>184150</xdr:rowOff>
+                    <xdr:rowOff>182880</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4099,15 +4844,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>4013200</xdr:colOff>
+                    <xdr:colOff>4015740</xdr:colOff>
                     <xdr:row>25</xdr:row>
-                    <xdr:rowOff>69850</xdr:rowOff>
+                    <xdr:rowOff>68580</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>38100</xdr:colOff>
                     <xdr:row>25</xdr:row>
-                    <xdr:rowOff>285750</xdr:rowOff>
+                    <xdr:rowOff>289560</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4123,13 +4868,13 @@
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>27</xdr:row>
-                    <xdr:rowOff>222250</xdr:rowOff>
+                    <xdr:rowOff>220980</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>50800</xdr:colOff>
+                    <xdr:colOff>53340</xdr:colOff>
                     <xdr:row>27</xdr:row>
-                    <xdr:rowOff>368300</xdr:rowOff>
+                    <xdr:rowOff>365760</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4145,13 +4890,13 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>4000500</xdr:colOff>
                     <xdr:row>28</xdr:row>
-                    <xdr:rowOff>107950</xdr:rowOff>
+                    <xdr:rowOff>106680</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>50800</xdr:colOff>
+                    <xdr:colOff>53340</xdr:colOff>
                     <xdr:row>28</xdr:row>
-                    <xdr:rowOff>323850</xdr:rowOff>
+                    <xdr:rowOff>327660</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4165,15 +4910,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>4013200</xdr:colOff>
+                    <xdr:colOff>4015740</xdr:colOff>
                     <xdr:row>29</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>50800</xdr:colOff>
-                    <xdr:row>30</xdr:row>
-                    <xdr:rowOff>31750</xdr:rowOff>
+                    <xdr:colOff>53340</xdr:colOff>
+                    <xdr:row>29</xdr:row>
+                    <xdr:rowOff>213360</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4187,15 +4932,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>4013200</xdr:colOff>
+                    <xdr:colOff>4015740</xdr:colOff>
                     <xdr:row>29</xdr:row>
                     <xdr:rowOff>190500</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>38100</xdr:colOff>
-                    <xdr:row>31</xdr:row>
-                    <xdr:rowOff>31750</xdr:rowOff>
+                    <xdr:row>30</xdr:row>
+                    <xdr:rowOff>38100</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4209,15 +4954,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>4013200</xdr:colOff>
-                    <xdr:row>31</xdr:row>
+                    <xdr:colOff>4015740</xdr:colOff>
+                    <xdr:row>32</xdr:row>
                     <xdr:rowOff>114300</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>50800</xdr:colOff>
-                    <xdr:row>31</xdr:row>
-                    <xdr:rowOff>336550</xdr:rowOff>
+                    <xdr:colOff>53340</xdr:colOff>
+                    <xdr:row>32</xdr:row>
+                    <xdr:rowOff>335280</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4231,15 +4976,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>4013200</xdr:colOff>
-                    <xdr:row>31</xdr:row>
+                    <xdr:colOff>4015740</xdr:colOff>
+                    <xdr:row>32</xdr:row>
                     <xdr:rowOff>381000</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>38100</xdr:colOff>
-                    <xdr:row>33</xdr:row>
-                    <xdr:rowOff>31750</xdr:rowOff>
+                    <xdr:row>35</xdr:row>
+                    <xdr:rowOff>30480</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4253,15 +4998,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>4013200</xdr:colOff>
-                    <xdr:row>34</xdr:row>
-                    <xdr:rowOff>209550</xdr:rowOff>
+                    <xdr:colOff>4015740</xdr:colOff>
+                    <xdr:row>35</xdr:row>
+                    <xdr:rowOff>213360</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>50800</xdr:colOff>
-                    <xdr:row>34</xdr:row>
-                    <xdr:rowOff>368300</xdr:rowOff>
+                    <xdr:colOff>53340</xdr:colOff>
+                    <xdr:row>36</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4275,15 +5020,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>4019550</xdr:colOff>
-                    <xdr:row>35</xdr:row>
-                    <xdr:rowOff>69850</xdr:rowOff>
+                    <xdr:colOff>4023360</xdr:colOff>
+                    <xdr:row>36</xdr:row>
+                    <xdr:rowOff>68580</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>44450</xdr:colOff>
-                    <xdr:row>35</xdr:row>
-                    <xdr:rowOff>184150</xdr:rowOff>
+                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:row>36</xdr:row>
+                    <xdr:rowOff>182880</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4298,14 +5043,14 @@
                   <from>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>36</xdr:row>
-                    <xdr:rowOff>95250</xdr:rowOff>
+                    <xdr:row>37</xdr:row>
+                    <xdr:rowOff>99060</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>38100</xdr:colOff>
-                    <xdr:row>36</xdr:row>
-                    <xdr:rowOff>292100</xdr:rowOff>
+                    <xdr:row>38</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4319,15 +5064,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>4013200</xdr:colOff>
-                    <xdr:row>37</xdr:row>
-                    <xdr:rowOff>57150</xdr:rowOff>
+                    <xdr:colOff>4015740</xdr:colOff>
+                    <xdr:row>38</xdr:row>
+                    <xdr:rowOff>60960</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>38100</xdr:colOff>
-                    <xdr:row>37</xdr:row>
-                    <xdr:rowOff>279400</xdr:rowOff>
+                    <xdr:row>38</xdr:row>
+                    <xdr:rowOff>281940</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4347,9 +5092,9 @@
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>50800</xdr:colOff>
+                    <xdr:colOff>53340</xdr:colOff>
                     <xdr:row>20</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:rowOff>22860</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4364,14 +5109,14 @@
                   <from>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>38</xdr:row>
+                    <xdr:row>39</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>50800</xdr:colOff>
-                    <xdr:row>39</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:colOff>53340</xdr:colOff>
+                    <xdr:row>40</xdr:row>
+                    <xdr:rowOff>22860</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4386,14 +5131,14 @@
                   <from>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>39</xdr:row>
-                    <xdr:rowOff>165100</xdr:rowOff>
+                    <xdr:row>40</xdr:row>
+                    <xdr:rowOff>167640</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>38100</xdr:colOff>
-                    <xdr:row>41</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:row>42</xdr:row>
+                    <xdr:rowOff>22860</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4408,14 +5153,14 @@
                   <from>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>46</xdr:row>
-                    <xdr:rowOff>165100</xdr:rowOff>
+                    <xdr:row>47</xdr:row>
+                    <xdr:rowOff>167640</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>38100</xdr:colOff>
-                    <xdr:row>47</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:row>48</xdr:row>
+                    <xdr:rowOff>22860</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4430,14 +5175,14 @@
                   <from>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>47</xdr:row>
-                    <xdr:rowOff>165100</xdr:rowOff>
+                    <xdr:row>48</xdr:row>
+                    <xdr:rowOff>167640</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>38100</xdr:colOff>
-                    <xdr:row>48</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:row>49</xdr:row>
+                    <xdr:rowOff>22860</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4459,7 +5204,7 @@
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>38100</xdr:colOff>
                     <xdr:row>21</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:rowOff>22860</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4474,14 +5219,14 @@
                   <from>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>41</xdr:row>
-                    <xdr:rowOff>139700</xdr:rowOff>
+                    <xdr:row>42</xdr:row>
+                    <xdr:rowOff>137160</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>38100</xdr:colOff>
-                    <xdr:row>41</xdr:row>
-                    <xdr:rowOff>336550</xdr:rowOff>
+                    <xdr:row>43</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4496,14 +5241,14 @@
                   <from>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>42</xdr:row>
-                    <xdr:rowOff>165100</xdr:rowOff>
+                    <xdr:row>43</xdr:row>
+                    <xdr:rowOff>167640</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>38100</xdr:colOff>
-                    <xdr:row>42</xdr:row>
-                    <xdr:rowOff>387350</xdr:rowOff>
+                    <xdr:row>43</xdr:row>
+                    <xdr:rowOff>388620</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4518,14 +5263,14 @@
                   <from>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>45</xdr:row>
-                    <xdr:rowOff>165100</xdr:rowOff>
+                    <xdr:row>46</xdr:row>
+                    <xdr:rowOff>167640</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>38100</xdr:colOff>
-                    <xdr:row>46</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:row>47</xdr:row>
+                    <xdr:rowOff>22860</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4540,14 +5285,14 @@
                   <from>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>43</xdr:row>
-                    <xdr:rowOff>165100</xdr:rowOff>
+                    <xdr:row>44</xdr:row>
+                    <xdr:rowOff>167640</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>38100</xdr:colOff>
-                    <xdr:row>44</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:row>45</xdr:row>
+                    <xdr:rowOff>22860</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4556,20 +5301,20 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1065" r:id="rId37" name="Check Box 41">
+            <control shapeId="1072" r:id="rId37" name="Check Box 48">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="_x000a_">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>2</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>49</xdr:row>
-                    <xdr:rowOff>165100</xdr:rowOff>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>4015740</xdr:colOff>
+                    <xdr:row>31</xdr:row>
+                    <xdr:rowOff>114300</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>38100</xdr:colOff>
-                    <xdr:row>49</xdr:row>
-                    <xdr:rowOff>393700</xdr:rowOff>
+                    <xdr:colOff>53340</xdr:colOff>
+                    <xdr:row>31</xdr:row>
+                    <xdr:rowOff>335280</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4578,20 +5323,152 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1066" r:id="rId38" name="Check Box 42">
+            <control shapeId="1073" r:id="rId38" name="Check Box 49">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="_x000a_">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>7620</xdr:colOff>
+                    <xdr:row>49</xdr:row>
+                    <xdr:rowOff>152400</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:row>51</xdr:row>
+                    <xdr:rowOff>7620</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1074" r:id="rId39" name="Check Box 50">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="_x000a_">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>15240</xdr:colOff>
+                    <xdr:row>50</xdr:row>
+                    <xdr:rowOff>175260</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>53340</xdr:colOff>
+                    <xdr:row>52</xdr:row>
+                    <xdr:rowOff>30480</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1075" r:id="rId40" name="Check Box 51">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="_x000a_">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>22860</xdr:colOff>
+                    <xdr:row>51</xdr:row>
+                    <xdr:rowOff>167640</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>60960</xdr:colOff>
+                    <xdr:row>53</xdr:row>
+                    <xdr:rowOff>22860</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1076" r:id="rId41" name="Check Box 52">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="_x000a_">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>45720</xdr:colOff>
+                    <xdr:row>52</xdr:row>
+                    <xdr:rowOff>175260</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>83820</xdr:colOff>
+                    <xdr:row>53</xdr:row>
+                    <xdr:rowOff>213360</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1078" r:id="rId42" name="Check Box 54">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="_x000a_">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>15240</xdr:colOff>
+                    <xdr:row>59</xdr:row>
+                    <xdr:rowOff>68580</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>53340</xdr:colOff>
+                    <xdr:row>59</xdr:row>
+                    <xdr:rowOff>289560</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1079" r:id="rId43" name="Check Box 55">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="_x000a_">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>51</xdr:row>
-                    <xdr:rowOff>165100</xdr:rowOff>
+                    <xdr:row>57</xdr:row>
+                    <xdr:rowOff>167640</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>38100</xdr:colOff>
-                    <xdr:row>51</xdr:row>
-                    <xdr:rowOff>387350</xdr:rowOff>
+                    <xdr:row>58</xdr:row>
+                    <xdr:rowOff>22860</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1080" r:id="rId44" name="Check Box 56">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="_x000a_">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>55</xdr:row>
+                    <xdr:rowOff>167640</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>38100</xdr:colOff>
+                    <xdr:row>55</xdr:row>
+                    <xdr:rowOff>388620</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>

</xml_diff>